<commit_message>
Rename data files (Part 4)
</commit_message>
<xml_diff>
--- a/data/regeco/IO Bungo 2010.xlsx
+++ b/data/regeco/IO Bungo 2010.xlsx
@@ -1,19 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ICRAF\Kodingan\icraf-indonesia\lumens-shiny\data\regeco\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFAF5BB-2B13-4919-97E2-9FF039157807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="72" windowWidth="20112" windowHeight="7992"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="IOBungo10" sheetId="6" r:id="rId1"/>
-    <sheet name="Permintaan_antara" sheetId="7" r:id="rId2"/>
-    <sheet name="Permintaan_akhir" sheetId="8" r:id="rId3"/>
-    <sheet name="Struktur_sektor" sheetId="9" r:id="rId4"/>
-    <sheet name="Nilai_tambah" sheetId="10" r:id="rId5"/>
-    <sheet name="Struktur_nilai_tambah" sheetId="11" r:id="rId6"/>
-    <sheet name="Struktur_permintaan_akhir" sheetId="12" r:id="rId7"/>
+    <sheet name="IO Bungo" sheetId="6" r:id="rId1"/>
+    <sheet name="Intermediate Demand" sheetId="7" r:id="rId2"/>
+    <sheet name="Sector" sheetId="9" r:id="rId3"/>
+    <sheet name="Added Value" sheetId="10" r:id="rId4"/>
+    <sheet name="Added Value Comp" sheetId="11" r:id="rId5"/>
+    <sheet name="Final Demand" sheetId="8" r:id="rId6"/>
+    <sheet name="Final Demand Comp" sheetId="12" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_Fill" localSheetId="0" hidden="1">#REF!</definedName>
@@ -24,12 +30,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="123">
   <si>
     <t>Bungo</t>
-  </si>
-  <si>
-    <t>Sektor Produksi</t>
   </si>
   <si>
     <t>Faktor Produksi</t>
@@ -182,19 +185,10 @@
     <t>Kegiatan yang tak jelas batasannya</t>
   </si>
   <si>
-    <t>Konsumsi Antara</t>
-  </si>
-  <si>
     <t>Investasi</t>
   </si>
   <si>
     <t>Ekspor</t>
-  </si>
-  <si>
-    <t>Pemintaan</t>
-  </si>
-  <si>
-    <t>Input Antara</t>
   </si>
   <si>
     <t>Impor</t>
@@ -203,13 +197,7 @@
     <t>201 sd 203</t>
   </si>
   <si>
-    <t>Input Primer</t>
-  </si>
-  <si>
     <t>Input</t>
-  </si>
-  <si>
-    <t>Tabel 1. IO Bungo Tahun 2010, 46 x 46 (Juta Rupiah)</t>
   </si>
   <si>
     <t>Pertanian</t>
@@ -235,18 +223,195 @@
   <si>
     <t>Lain-lain</t>
   </si>
+  <si>
+    <t>Tabel 1. IO Bungo District 2010, 46 x 46 (Million IDR)</t>
+  </si>
+  <si>
+    <t>Paddy</t>
+  </si>
+  <si>
+    <t>Tuber Crops</t>
+  </si>
+  <si>
+    <t>Vegetables and Fruits</t>
+  </si>
+  <si>
+    <t>Other Food Crops</t>
+  </si>
+  <si>
+    <t>Rubber</t>
+  </si>
+  <si>
+    <t>Coconut</t>
+  </si>
+  <si>
+    <t>Oil Palm</t>
+  </si>
+  <si>
+    <t>Coffee</t>
+  </si>
+  <si>
+    <t>Cinnamon</t>
+  </si>
+  <si>
+    <t>Other Plantation Crops</t>
+  </si>
+  <si>
+    <t>Livestock and Products</t>
+  </si>
+  <si>
+    <t>Roundwood</t>
+  </si>
+  <si>
+    <t>Industrial Plantation Forest Timber</t>
+  </si>
+  <si>
+    <t>Other Forest Products</t>
+  </si>
+  <si>
+    <t>Fisheries</t>
+  </si>
+  <si>
+    <t>Oil and Gas Mining</t>
+  </si>
+  <si>
+    <t>Coal Mining</t>
+  </si>
+  <si>
+    <t>Other Non-Oil and Gas Mining</t>
+  </si>
+  <si>
+    <t>Oil Refining</t>
+  </si>
+  <si>
+    <t>Seafood Processing Industry</t>
+  </si>
+  <si>
+    <t>Palm Oil Industry</t>
+  </si>
+  <si>
+    <t>Rice and Grain Milling Industry</t>
+  </si>
+  <si>
+    <t>Other Food and Beverage Industry</t>
+  </si>
+  <si>
+    <t>Textile, Leather Goods, and Footwear Industry</t>
+  </si>
+  <si>
+    <t>Wood Products and Other Forest Products Industry</t>
+  </si>
+  <si>
+    <t>Paper and Paper Products Industry</t>
+  </si>
+  <si>
+    <t>Fertilizer, Chemical, and Rubber Products Industry</t>
+  </si>
+  <si>
+    <t>Cement and Non-Metal Mineral Products Industry</t>
+  </si>
+  <si>
+    <t>Transportation Equipment and Machinery Industry</t>
+  </si>
+  <si>
+    <t>Other Goods Industry</t>
+  </si>
+  <si>
+    <t>Electricity and Drinking Water</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Trade</t>
+  </si>
+  <si>
+    <t>Restaurants and Hotels</t>
+  </si>
+  <si>
+    <t>Road Transport</t>
+  </si>
+  <si>
+    <t>Sea Transport</t>
+  </si>
+  <si>
+    <t>River and Lake Transport</t>
+  </si>
+  <si>
+    <t>Air Transport</t>
+  </si>
+  <si>
+    <t>Transportation Support Services</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>Banks and Financial Institutions</t>
+  </si>
+  <si>
+    <t>Construction and Business Services</t>
+  </si>
+  <si>
+    <t>General Government and Defense</t>
+  </si>
+  <si>
+    <t>Social Community Services</t>
+  </si>
+  <si>
+    <t>Other Services</t>
+  </si>
+  <si>
+    <t>Undefined Activities</t>
+  </si>
+  <si>
+    <t>Intermediate Demand</t>
+  </si>
+  <si>
+    <t>Import</t>
+  </si>
+  <si>
+    <t>Factors of Production</t>
+  </si>
+  <si>
+    <t>Net Indirect Taxes</t>
+  </si>
+  <si>
+    <t>Primary Input</t>
+  </si>
+  <si>
+    <t>Households</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>Investment</t>
+  </si>
+  <si>
+    <t>Export</t>
+  </si>
+  <si>
+    <t>Demand</t>
+  </si>
+  <si>
+    <t>Production Sectors</t>
+  </si>
+  <si>
+    <t>Intermediate Consumption</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0_);\(0\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="0_);\(0\)"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -520,21 +685,21 @@
   </borders>
   <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="5" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -574,7 +739,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="40" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -585,14 +750,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -610,7 +775,7 @@
     <xf numFmtId="40" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="8" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="8" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -632,10 +797,9 @@
     <xf numFmtId="40" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="40" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="40" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -650,8 +814,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -670,7 +834,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -700,31 +864,22 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0] 2" xfId="3"/>
-    <cellStyle name="Comma [0] 3" xfId="4"/>
-    <cellStyle name="Comma 2" xfId="5"/>
-    <cellStyle name="Comma 3" xfId="6"/>
-    <cellStyle name="Comma 4" xfId="7"/>
-    <cellStyle name="Comma0" xfId="8"/>
-    <cellStyle name="Currency0" xfId="9"/>
-    <cellStyle name="Date" xfId="10"/>
-    <cellStyle name="Fixed" xfId="11"/>
+    <cellStyle name="Comma [0] 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Comma [0] 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Comma 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Comma 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Comma 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Comma0" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Currency0" xfId="9" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Date" xfId="10" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Fixed" xfId="11" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="12"/>
-    <cellStyle name="Normal 3" xfId="13"/>
-    <cellStyle name="Normal 4" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal 3" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -732,14 +887,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -777,7 +935,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -811,6 +969,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -845,9 +1004,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1020,20 +1180,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:BT75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="9" topLeftCell="AX45" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="6" ySplit="9" topLeftCell="G25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="BB6" sqref="BB6:BE8"/>
+      <selection pane="bottomRight" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="36.33203125" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="36.33203125" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.44140625" style="10" customWidth="1"/>
     <col min="2" max="3" width="7.109375" style="10" customWidth="1"/>
@@ -1047,9 +1207,9 @@
     <col min="65" max="16384" width="36.33203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:72" s="1" customFormat="1" ht="28.8">
+    <row r="1" spans="1:72" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D1" s="2"/>
       <c r="F1" s="3"/>
@@ -1103,7 +1263,7 @@
       <c r="BB1" s="4"/>
       <c r="BC1" s="4"/>
     </row>
-    <row r="5" spans="1:72" s="5" customFormat="1">
+    <row r="5" spans="1:72" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D5" s="6"/>
       <c r="F5" s="7"/>
       <c r="G5" s="8"/>
@@ -1156,239 +1316,239 @@
       <c r="BB5" s="8"/>
       <c r="BC5" s="8"/>
     </row>
-    <row r="6" spans="1:72" s="5" customFormat="1" ht="18" customHeight="1">
-      <c r="A6" s="59"/>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" s="63"/>
-      <c r="I6" s="63"/>
-      <c r="J6" s="63"/>
-      <c r="K6" s="63"/>
-      <c r="L6" s="63"/>
-      <c r="M6" s="63"/>
-      <c r="N6" s="63"/>
-      <c r="O6" s="63"/>
-      <c r="P6" s="63"/>
-      <c r="Q6" s="63"/>
-      <c r="R6" s="63"/>
-      <c r="S6" s="63"/>
-      <c r="T6" s="63"/>
-      <c r="U6" s="63"/>
-      <c r="V6" s="63"/>
-      <c r="W6" s="63"/>
-      <c r="X6" s="63"/>
-      <c r="Y6" s="63"/>
-      <c r="Z6" s="63"/>
-      <c r="AA6" s="63"/>
-      <c r="AB6" s="63"/>
-      <c r="AC6" s="63"/>
-      <c r="AD6" s="63"/>
-      <c r="AE6" s="63"/>
-      <c r="AF6" s="63"/>
-      <c r="AG6" s="63"/>
-      <c r="AH6" s="63"/>
-      <c r="AI6" s="63"/>
-      <c r="AJ6" s="63"/>
-      <c r="AK6" s="63"/>
-      <c r="AL6" s="63"/>
-      <c r="AM6" s="63"/>
-      <c r="AN6" s="63"/>
-      <c r="AO6" s="63"/>
-      <c r="AP6" s="63"/>
-      <c r="AQ6" s="63"/>
-      <c r="AR6" s="63"/>
-      <c r="AS6" s="63"/>
-      <c r="AT6" s="63"/>
-      <c r="AU6" s="63"/>
-      <c r="AV6" s="63"/>
-      <c r="AW6" s="63"/>
-      <c r="AX6" s="63"/>
-      <c r="AY6" s="63"/>
-      <c r="AZ6" s="63"/>
-      <c r="BA6" s="64" t="s">
-        <v>52</v>
-      </c>
-      <c r="BB6" s="67" t="s">
-        <v>3</v>
-      </c>
-      <c r="BC6" s="67" t="s">
-        <v>4</v>
-      </c>
-      <c r="BD6" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="BE6" s="51" t="s">
-        <v>54</v>
-      </c>
-      <c r="BF6" s="51" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:72" s="5" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A7" s="59"/>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="60"/>
+    <row r="6" spans="1:72" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="58"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="62"/>
+      <c r="N6" s="62"/>
+      <c r="O6" s="62"/>
+      <c r="P6" s="62"/>
+      <c r="Q6" s="62"/>
+      <c r="R6" s="62"/>
+      <c r="S6" s="62"/>
+      <c r="T6" s="62"/>
+      <c r="U6" s="62"/>
+      <c r="V6" s="62"/>
+      <c r="W6" s="62"/>
+      <c r="X6" s="62"/>
+      <c r="Y6" s="62"/>
+      <c r="Z6" s="62"/>
+      <c r="AA6" s="62"/>
+      <c r="AB6" s="62"/>
+      <c r="AC6" s="62"/>
+      <c r="AD6" s="62"/>
+      <c r="AE6" s="62"/>
+      <c r="AF6" s="62"/>
+      <c r="AG6" s="62"/>
+      <c r="AH6" s="62"/>
+      <c r="AI6" s="62"/>
+      <c r="AJ6" s="62"/>
+      <c r="AK6" s="62"/>
+      <c r="AL6" s="62"/>
+      <c r="AM6" s="62"/>
+      <c r="AN6" s="62"/>
+      <c r="AO6" s="62"/>
+      <c r="AP6" s="62"/>
+      <c r="AQ6" s="62"/>
+      <c r="AR6" s="62"/>
+      <c r="AS6" s="62"/>
+      <c r="AT6" s="62"/>
+      <c r="AU6" s="62"/>
+      <c r="AV6" s="62"/>
+      <c r="AW6" s="62"/>
+      <c r="AX6" s="62"/>
+      <c r="AY6" s="62"/>
+      <c r="AZ6" s="62"/>
+      <c r="BA6" s="63" t="s">
+        <v>122</v>
+      </c>
+      <c r="BB6" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="BC6" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD6" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="BE6" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="BF6" s="50" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:72" s="5" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="58"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="59"/>
       <c r="G7" s="9" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="P7" s="9" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="S7" s="9" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="T7" s="9" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="U7" s="9" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="V7" s="9" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="W7" s="9" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="X7" s="9" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="Y7" s="9" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="Z7" s="9" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="AA7" s="9" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="AB7" s="9" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="AC7" s="9" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="AD7" s="9" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="AE7" s="9" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="AF7" s="9" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="AG7" s="9" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
       <c r="AH7" s="9" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="AI7" s="9" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="AJ7" s="9" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="AK7" s="9" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="AL7" s="9" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="AM7" s="9" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="AN7" s="9" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="AO7" s="9" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="AP7" s="9" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="AQ7" s="9" t="s">
-        <v>42</v>
+        <v>101</v>
       </c>
       <c r="AR7" s="9" t="s">
-        <v>43</v>
+        <v>102</v>
       </c>
       <c r="AS7" s="9" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="AT7" s="9" t="s">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="AU7" s="9" t="s">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="AV7" s="9" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="AW7" s="9" t="s">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="AX7" s="9" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="AY7" s="9" t="s">
-        <v>50</v>
+        <v>109</v>
       </c>
       <c r="AZ7" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="BA7" s="65"/>
-      <c r="BB7" s="68"/>
-      <c r="BC7" s="68"/>
-      <c r="BD7" s="52"/>
-      <c r="BE7" s="52"/>
-      <c r="BF7" s="52"/>
-    </row>
-    <row r="8" spans="1:72" s="5" customFormat="1">
-      <c r="A8" s="59"/>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="60"/>
+        <v>110</v>
+      </c>
+      <c r="BA7" s="64"/>
+      <c r="BB7" s="51"/>
+      <c r="BC7" s="51"/>
+      <c r="BD7" s="51"/>
+      <c r="BE7" s="51"/>
+      <c r="BF7" s="51"/>
+    </row>
+    <row r="8" spans="1:72" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="58"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="59"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -1435,20 +1595,20 @@
       <c r="AX8" s="9"/>
       <c r="AY8" s="9"/>
       <c r="AZ8" s="9"/>
-      <c r="BA8" s="66"/>
-      <c r="BB8" s="69"/>
-      <c r="BC8" s="69"/>
-      <c r="BD8" s="53"/>
-      <c r="BE8" s="53"/>
-      <c r="BF8" s="53"/>
-    </row>
-    <row r="9" spans="1:72" s="5" customFormat="1">
-      <c r="A9" s="61"/>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="62"/>
+      <c r="BA8" s="65"/>
+      <c r="BB8" s="52"/>
+      <c r="BC8" s="52"/>
+      <c r="BD8" s="52"/>
+      <c r="BE8" s="52"/>
+      <c r="BF8" s="52"/>
+    </row>
+    <row r="9" spans="1:72" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="60"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="61"/>
       <c r="G9" s="9">
         <v>1</v>
       </c>
@@ -1620,16 +1780,16 @@
       <c r="BS9" s="10"/>
       <c r="BT9" s="10"/>
     </row>
-    <row r="10" spans="1:72" ht="12.75" customHeight="1">
-      <c r="A10" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="57"/>
+    <row r="10" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="56"/>
       <c r="D10" s="11" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="13">
@@ -1794,12 +1954,12 @@
       <c r="BG10" s="16"/>
       <c r="BI10" s="17"/>
     </row>
-    <row r="11" spans="1:72">
-      <c r="A11" s="55"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
+    <row r="11" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A11" s="54"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
       <c r="D11" s="11" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="18">
@@ -1964,12 +2124,12 @@
       <c r="BG11" s="16"/>
       <c r="BI11" s="17"/>
     </row>
-    <row r="12" spans="1:72">
-      <c r="A12" s="55"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
+    <row r="12" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A12" s="54"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
       <c r="D12" s="11" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="18">
@@ -2134,12 +2294,12 @@
       <c r="BG12" s="16"/>
       <c r="BI12" s="17"/>
     </row>
-    <row r="13" spans="1:72">
-      <c r="A13" s="55"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
+    <row r="13" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A13" s="54"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
       <c r="D13" s="11" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="18">
@@ -2304,12 +2464,12 @@
       <c r="BG13" s="16"/>
       <c r="BI13" s="17"/>
     </row>
-    <row r="14" spans="1:72">
-      <c r="A14" s="55"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
+    <row r="14" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A14" s="54"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
       <c r="D14" s="11" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="18">
@@ -2474,12 +2634,12 @@
       <c r="BG14" s="16"/>
       <c r="BI14" s="17"/>
     </row>
-    <row r="15" spans="1:72">
-      <c r="A15" s="55"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
+    <row r="15" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A15" s="54"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
       <c r="D15" s="11" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="18">
@@ -2644,12 +2804,12 @@
       <c r="BG15" s="16"/>
       <c r="BI15" s="17"/>
     </row>
-    <row r="16" spans="1:72">
-      <c r="A16" s="55"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
+    <row r="16" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A16" s="54"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
       <c r="D16" s="11" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="18">
@@ -2814,12 +2974,12 @@
       <c r="BG16" s="16"/>
       <c r="BI16" s="17"/>
     </row>
-    <row r="17" spans="1:61">
-      <c r="A17" s="55"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
+    <row r="17" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A17" s="54"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
       <c r="D17" s="11" t="s">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="18">
@@ -2984,12 +3144,12 @@
       <c r="BG17" s="16"/>
       <c r="BI17" s="17"/>
     </row>
-    <row r="18" spans="1:61">
-      <c r="A18" s="55"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
+    <row r="18" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A18" s="54"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
       <c r="D18" s="11" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="18">
@@ -3154,12 +3314,12 @@
       <c r="BG18" s="16"/>
       <c r="BI18" s="17"/>
     </row>
-    <row r="19" spans="1:61">
-      <c r="A19" s="55"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
+    <row r="19" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A19" s="54"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
       <c r="D19" s="11" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="18">
@@ -3324,12 +3484,12 @@
       <c r="BG19" s="16"/>
       <c r="BI19" s="17"/>
     </row>
-    <row r="20" spans="1:61">
-      <c r="A20" s="55"/>
-      <c r="B20" s="57"/>
-      <c r="C20" s="57"/>
+    <row r="20" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A20" s="54"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
       <c r="D20" s="11" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="E20" s="12"/>
       <c r="F20" s="18">
@@ -3494,12 +3654,12 @@
       <c r="BG20" s="16"/>
       <c r="BI20" s="17"/>
     </row>
-    <row r="21" spans="1:61">
-      <c r="A21" s="55"/>
-      <c r="B21" s="57"/>
-      <c r="C21" s="57"/>
+    <row r="21" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A21" s="54"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
       <c r="D21" s="11" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="E21" s="12"/>
       <c r="F21" s="18">
@@ -3664,12 +3824,12 @@
       <c r="BG21" s="16"/>
       <c r="BI21" s="17"/>
     </row>
-    <row r="22" spans="1:61">
-      <c r="A22" s="55"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="57"/>
+    <row r="22" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A22" s="54"/>
+      <c r="B22" s="56"/>
+      <c r="C22" s="56"/>
       <c r="D22" s="11" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="E22" s="12"/>
       <c r="F22" s="18">
@@ -3834,12 +3994,12 @@
       <c r="BG22" s="16"/>
       <c r="BI22" s="17"/>
     </row>
-    <row r="23" spans="1:61">
-      <c r="A23" s="55"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
+    <row r="23" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A23" s="54"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56"/>
       <c r="D23" s="11" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="18">
@@ -4004,12 +4164,12 @@
       <c r="BG23" s="16"/>
       <c r="BI23" s="17"/>
     </row>
-    <row r="24" spans="1:61">
-      <c r="A24" s="55"/>
-      <c r="B24" s="57"/>
-      <c r="C24" s="57"/>
+    <row r="24" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A24" s="54"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="56"/>
       <c r="D24" s="11" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="E24" s="12"/>
       <c r="F24" s="18">
@@ -4174,12 +4334,12 @@
       <c r="BG24" s="16"/>
       <c r="BI24" s="17"/>
     </row>
-    <row r="25" spans="1:61">
-      <c r="A25" s="55"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
+    <row r="25" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A25" s="54"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
       <c r="D25" s="11" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="E25" s="12"/>
       <c r="F25" s="18">
@@ -4344,12 +4504,12 @@
       <c r="BG25" s="16"/>
       <c r="BI25" s="17"/>
     </row>
-    <row r="26" spans="1:61">
-      <c r="A26" s="55"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
+    <row r="26" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A26" s="54"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="56"/>
       <c r="D26" s="11" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="E26" s="12"/>
       <c r="F26" s="18">
@@ -4514,12 +4674,12 @@
       <c r="BG26" s="16"/>
       <c r="BI26" s="17"/>
     </row>
-    <row r="27" spans="1:61">
-      <c r="A27" s="55"/>
-      <c r="B27" s="57"/>
-      <c r="C27" s="57"/>
+    <row r="27" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A27" s="54"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="56"/>
       <c r="D27" s="11" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="E27" s="12"/>
       <c r="F27" s="18">
@@ -4684,12 +4844,12 @@
       <c r="BG27" s="16"/>
       <c r="BI27" s="17"/>
     </row>
-    <row r="28" spans="1:61">
-      <c r="A28" s="55"/>
-      <c r="B28" s="57"/>
-      <c r="C28" s="57"/>
+    <row r="28" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A28" s="54"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="56"/>
       <c r="D28" s="11" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="E28" s="12"/>
       <c r="F28" s="18">
@@ -4854,12 +5014,12 @@
       <c r="BG28" s="16"/>
       <c r="BI28" s="17"/>
     </row>
-    <row r="29" spans="1:61">
-      <c r="A29" s="55"/>
-      <c r="B29" s="57"/>
-      <c r="C29" s="57"/>
+    <row r="29" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A29" s="54"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="56"/>
       <c r="D29" s="11" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="18">
@@ -5024,12 +5184,12 @@
       <c r="BG29" s="16"/>
       <c r="BI29" s="17"/>
     </row>
-    <row r="30" spans="1:61">
-      <c r="A30" s="55"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="57"/>
+    <row r="30" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A30" s="54"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
       <c r="D30" s="11" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="E30" s="12"/>
       <c r="F30" s="18">
@@ -5194,12 +5354,12 @@
       <c r="BG30" s="16"/>
       <c r="BI30" s="17"/>
     </row>
-    <row r="31" spans="1:61">
-      <c r="A31" s="55"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="57"/>
+    <row r="31" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A31" s="54"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
       <c r="D31" s="11" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="E31" s="12"/>
       <c r="F31" s="18">
@@ -5364,12 +5524,12 @@
       <c r="BG31" s="16"/>
       <c r="BI31" s="17"/>
     </row>
-    <row r="32" spans="1:61">
-      <c r="A32" s="55"/>
-      <c r="B32" s="57"/>
-      <c r="C32" s="57"/>
+    <row r="32" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A32" s="54"/>
+      <c r="B32" s="56"/>
+      <c r="C32" s="56"/>
       <c r="D32" s="11" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="18">
@@ -5534,12 +5694,12 @@
       <c r="BG32" s="16"/>
       <c r="BI32" s="17"/>
     </row>
-    <row r="33" spans="1:61">
-      <c r="A33" s="55"/>
-      <c r="B33" s="57"/>
-      <c r="C33" s="57"/>
+    <row r="33" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A33" s="54"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="56"/>
       <c r="D33" s="11" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="18">
@@ -5704,12 +5864,12 @@
       <c r="BG33" s="16"/>
       <c r="BI33" s="17"/>
     </row>
-    <row r="34" spans="1:61">
-      <c r="A34" s="55"/>
-      <c r="B34" s="57"/>
-      <c r="C34" s="57"/>
+    <row r="34" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A34" s="54"/>
+      <c r="B34" s="56"/>
+      <c r="C34" s="56"/>
       <c r="D34" s="11" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="18">
@@ -5869,17 +6029,17 @@
         <v>593688.57871703629</v>
       </c>
       <c r="BF34" s="33">
-        <v>540406.8517272356</v>
+        <v>540406.85172723595</v>
       </c>
       <c r="BG34" s="16"/>
       <c r="BI34" s="17"/>
     </row>
-    <row r="35" spans="1:61">
-      <c r="A35" s="55"/>
-      <c r="B35" s="57"/>
-      <c r="C35" s="57"/>
+    <row r="35" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A35" s="54"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="56"/>
       <c r="D35" s="11" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="18">
@@ -6044,12 +6204,12 @@
       <c r="BG35" s="16"/>
       <c r="BI35" s="17"/>
     </row>
-    <row r="36" spans="1:61">
-      <c r="A36" s="55"/>
-      <c r="B36" s="57"/>
-      <c r="C36" s="57"/>
+    <row r="36" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A36" s="54"/>
+      <c r="B36" s="56"/>
+      <c r="C36" s="56"/>
       <c r="D36" s="11" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
       <c r="E36" s="12"/>
       <c r="F36" s="18">
@@ -6214,12 +6374,12 @@
       <c r="BG36" s="16"/>
       <c r="BI36" s="17"/>
     </row>
-    <row r="37" spans="1:61">
-      <c r="A37" s="55"/>
-      <c r="B37" s="57"/>
-      <c r="C37" s="57"/>
+    <row r="37" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A37" s="54"/>
+      <c r="B37" s="56"/>
+      <c r="C37" s="56"/>
       <c r="D37" s="11" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="E37" s="12"/>
       <c r="F37" s="18">
@@ -6384,12 +6544,12 @@
       <c r="BG37" s="16"/>
       <c r="BI37" s="17"/>
     </row>
-    <row r="38" spans="1:61">
-      <c r="A38" s="55"/>
-      <c r="B38" s="57"/>
-      <c r="C38" s="57"/>
+    <row r="38" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A38" s="54"/>
+      <c r="B38" s="56"/>
+      <c r="C38" s="56"/>
       <c r="D38" s="11" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="E38" s="12"/>
       <c r="F38" s="18">
@@ -6554,12 +6714,12 @@
       <c r="BG38" s="16"/>
       <c r="BI38" s="17"/>
     </row>
-    <row r="39" spans="1:61">
-      <c r="A39" s="55"/>
-      <c r="B39" s="57"/>
-      <c r="C39" s="57"/>
+    <row r="39" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A39" s="54"/>
+      <c r="B39" s="56"/>
+      <c r="C39" s="56"/>
       <c r="D39" s="11" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="E39" s="12"/>
       <c r="F39" s="18">
@@ -6724,12 +6884,12 @@
       <c r="BG39" s="16"/>
       <c r="BI39" s="17"/>
     </row>
-    <row r="40" spans="1:61">
-      <c r="A40" s="55"/>
-      <c r="B40" s="57"/>
-      <c r="C40" s="57"/>
+    <row r="40" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A40" s="54"/>
+      <c r="B40" s="56"/>
+      <c r="C40" s="56"/>
       <c r="D40" s="11" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="E40" s="12"/>
       <c r="F40" s="18">
@@ -6894,12 +7054,12 @@
       <c r="BG40" s="16"/>
       <c r="BI40" s="17"/>
     </row>
-    <row r="41" spans="1:61">
-      <c r="A41" s="55"/>
-      <c r="B41" s="57"/>
-      <c r="C41" s="57"/>
+    <row r="41" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A41" s="54"/>
+      <c r="B41" s="56"/>
+      <c r="C41" s="56"/>
       <c r="D41" s="11" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="E41" s="12"/>
       <c r="F41" s="18">
@@ -7064,12 +7224,12 @@
       <c r="BG41" s="16"/>
       <c r="BI41" s="17"/>
     </row>
-    <row r="42" spans="1:61">
-      <c r="A42" s="55"/>
-      <c r="B42" s="57"/>
-      <c r="C42" s="57"/>
+    <row r="42" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A42" s="54"/>
+      <c r="B42" s="56"/>
+      <c r="C42" s="56"/>
       <c r="D42" s="11" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="E42" s="12"/>
       <c r="F42" s="18">
@@ -7234,12 +7394,12 @@
       <c r="BG42" s="16"/>
       <c r="BI42" s="17"/>
     </row>
-    <row r="43" spans="1:61">
-      <c r="A43" s="55"/>
-      <c r="B43" s="57"/>
-      <c r="C43" s="57"/>
+    <row r="43" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A43" s="54"/>
+      <c r="B43" s="56"/>
+      <c r="C43" s="56"/>
       <c r="D43" s="11" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="E43" s="12"/>
       <c r="F43" s="18">
@@ -7404,12 +7564,12 @@
       <c r="BG43" s="16"/>
       <c r="BI43" s="17"/>
     </row>
-    <row r="44" spans="1:61">
-      <c r="A44" s="55"/>
-      <c r="B44" s="57"/>
-      <c r="C44" s="57"/>
+    <row r="44" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A44" s="54"/>
+      <c r="B44" s="56"/>
+      <c r="C44" s="56"/>
       <c r="D44" s="11" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="E44" s="12"/>
       <c r="F44" s="18">
@@ -7574,12 +7734,12 @@
       <c r="BG44" s="16"/>
       <c r="BI44" s="17"/>
     </row>
-    <row r="45" spans="1:61">
-      <c r="A45" s="55"/>
-      <c r="B45" s="57"/>
-      <c r="C45" s="57"/>
+    <row r="45" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A45" s="54"/>
+      <c r="B45" s="56"/>
+      <c r="C45" s="56"/>
       <c r="D45" s="11" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="E45" s="12"/>
       <c r="F45" s="18">
@@ -7744,12 +7904,12 @@
       <c r="BG45" s="16"/>
       <c r="BI45" s="17"/>
     </row>
-    <row r="46" spans="1:61">
-      <c r="A46" s="55"/>
-      <c r="B46" s="57"/>
-      <c r="C46" s="57"/>
+    <row r="46" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A46" s="54"/>
+      <c r="B46" s="56"/>
+      <c r="C46" s="56"/>
       <c r="D46" s="11" t="s">
-        <v>42</v>
+        <v>101</v>
       </c>
       <c r="E46" s="12"/>
       <c r="F46" s="18">
@@ -7914,12 +8074,12 @@
       <c r="BG46" s="16"/>
       <c r="BI46" s="17"/>
     </row>
-    <row r="47" spans="1:61">
-      <c r="A47" s="55"/>
-      <c r="B47" s="57"/>
-      <c r="C47" s="57"/>
+    <row r="47" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A47" s="54"/>
+      <c r="B47" s="56"/>
+      <c r="C47" s="56"/>
       <c r="D47" s="11" t="s">
-        <v>43</v>
+        <v>102</v>
       </c>
       <c r="E47" s="12"/>
       <c r="F47" s="18">
@@ -8084,12 +8244,12 @@
       <c r="BG47" s="16"/>
       <c r="BI47" s="17"/>
     </row>
-    <row r="48" spans="1:61">
-      <c r="A48" s="55"/>
-      <c r="B48" s="57"/>
-      <c r="C48" s="57"/>
+    <row r="48" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A48" s="54"/>
+      <c r="B48" s="56"/>
+      <c r="C48" s="56"/>
       <c r="D48" s="11" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="E48" s="12"/>
       <c r="F48" s="18">
@@ -8254,12 +8414,12 @@
       <c r="BG48" s="16"/>
       <c r="BI48" s="17"/>
     </row>
-    <row r="49" spans="1:61">
-      <c r="A49" s="55"/>
-      <c r="B49" s="57"/>
-      <c r="C49" s="57"/>
+    <row r="49" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A49" s="54"/>
+      <c r="B49" s="56"/>
+      <c r="C49" s="56"/>
       <c r="D49" s="11" t="s">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="E49" s="12"/>
       <c r="F49" s="18">
@@ -8424,12 +8584,12 @@
       <c r="BG49" s="16"/>
       <c r="BI49" s="17"/>
     </row>
-    <row r="50" spans="1:61">
-      <c r="A50" s="55"/>
-      <c r="B50" s="57"/>
-      <c r="C50" s="57"/>
+    <row r="50" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A50" s="54"/>
+      <c r="B50" s="56"/>
+      <c r="C50" s="56"/>
       <c r="D50" s="11" t="s">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="E50" s="12"/>
       <c r="F50" s="18">
@@ -8594,12 +8754,12 @@
       <c r="BG50" s="16"/>
       <c r="BI50" s="17"/>
     </row>
-    <row r="51" spans="1:61">
-      <c r="A51" s="55"/>
-      <c r="B51" s="57"/>
-      <c r="C51" s="57"/>
+    <row r="51" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A51" s="54"/>
+      <c r="B51" s="56"/>
+      <c r="C51" s="56"/>
       <c r="D51" s="11" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="E51" s="12"/>
       <c r="F51" s="18">
@@ -8764,12 +8924,12 @@
       <c r="BG51" s="16"/>
       <c r="BI51" s="17"/>
     </row>
-    <row r="52" spans="1:61">
-      <c r="A52" s="55"/>
-      <c r="B52" s="57"/>
-      <c r="C52" s="57"/>
+    <row r="52" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A52" s="54"/>
+      <c r="B52" s="56"/>
+      <c r="C52" s="56"/>
       <c r="D52" s="11" t="s">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="E52" s="12"/>
       <c r="F52" s="18">
@@ -8934,12 +9094,12 @@
       <c r="BG52" s="16"/>
       <c r="BI52" s="17"/>
     </row>
-    <row r="53" spans="1:61">
-      <c r="A53" s="55"/>
-      <c r="B53" s="57"/>
-      <c r="C53" s="57"/>
+    <row r="53" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A53" s="54"/>
+      <c r="B53" s="56"/>
+      <c r="C53" s="56"/>
       <c r="D53" s="11" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="E53" s="12"/>
       <c r="F53" s="18">
@@ -9104,12 +9264,12 @@
       <c r="BG53" s="16"/>
       <c r="BI53" s="17"/>
     </row>
-    <row r="54" spans="1:61">
-      <c r="A54" s="55"/>
-      <c r="B54" s="57"/>
-      <c r="C54" s="57"/>
+    <row r="54" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A54" s="54"/>
+      <c r="B54" s="56"/>
+      <c r="C54" s="56"/>
       <c r="D54" s="11" t="s">
-        <v>50</v>
+        <v>109</v>
       </c>
       <c r="E54" s="12"/>
       <c r="F54" s="18">
@@ -9274,12 +9434,12 @@
       <c r="BG54" s="16"/>
       <c r="BI54" s="17"/>
     </row>
-    <row r="55" spans="1:61">
-      <c r="A55" s="55"/>
-      <c r="B55" s="58"/>
-      <c r="C55" s="58"/>
+    <row r="55" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A55" s="54"/>
+      <c r="B55" s="57"/>
+      <c r="C55" s="57"/>
       <c r="D55" s="19" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
       <c r="E55" s="20"/>
       <c r="F55" s="34">
@@ -9444,10 +9604,10 @@
       <c r="BG55" s="16"/>
       <c r="BI55" s="17"/>
     </row>
-    <row r="56" spans="1:61">
-      <c r="A56" s="55"/>
+    <row r="56" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A56" s="54"/>
       <c r="B56" s="36" t="s">
-        <v>56</v>
+        <v>111</v>
       </c>
       <c r="C56" s="37"/>
       <c r="D56" s="37"/>
@@ -9614,10 +9774,10 @@
       <c r="BG56" s="16"/>
       <c r="BI56" s="17"/>
     </row>
-    <row r="57" spans="1:61" ht="12.75" customHeight="1">
-      <c r="A57" s="55"/>
+    <row r="57" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="54"/>
       <c r="B57" s="36" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
       <c r="C57" s="37"/>
       <c r="D57" s="37"/>
@@ -9770,20 +9930,19 @@
       <c r="BC57" s="41"/>
       <c r="BD57" s="41"/>
       <c r="BE57" s="41"/>
-      <c r="BF57" s="42"/>
       <c r="BG57" s="16"/>
       <c r="BI57" s="17"/>
     </row>
-    <row r="58" spans="1:61" ht="12.75" customHeight="1">
-      <c r="A58" s="55"/>
-      <c r="B58" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="C58" s="44"/>
-      <c r="D58" s="44"/>
-      <c r="E58" s="45"/>
+    <row r="58" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="54"/>
+      <c r="B58" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="C58" s="43"/>
+      <c r="D58" s="43"/>
+      <c r="E58" s="44"/>
       <c r="F58" s="18" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G58" s="14">
         <v>1844809.6525243714</v>
@@ -9930,16 +10089,15 @@
       <c r="BC58" s="41"/>
       <c r="BD58" s="41"/>
       <c r="BE58" s="41"/>
-      <c r="BF58" s="42"/>
       <c r="BG58" s="16"/>
       <c r="BI58" s="17"/>
     </row>
-    <row r="59" spans="1:61">
-      <c r="A59" s="55"/>
+    <row r="59" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A59" s="54"/>
       <c r="B59" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="46"/>
+        <v>114</v>
+      </c>
+      <c r="C59" s="45"/>
       <c r="D59" s="22"/>
       <c r="E59" s="23"/>
       <c r="F59" s="34">
@@ -10089,13 +10247,13 @@
       <c r="BB59" s="10"/>
       <c r="BC59" s="17"/>
     </row>
-    <row r="60" spans="1:61">
-      <c r="A60" s="55"/>
-      <c r="B60" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="C60" s="46"/>
-      <c r="D60" s="48"/>
+    <row r="60" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A60" s="54"/>
+      <c r="B60" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="C60" s="45"/>
+      <c r="D60" s="47"/>
       <c r="E60" s="23"/>
       <c r="F60" s="18">
         <v>209</v>
@@ -10244,15 +10402,15 @@
       <c r="BB60" s="10"/>
       <c r="BC60" s="17"/>
     </row>
-    <row r="61" spans="1:61" s="26" customFormat="1">
-      <c r="A61" s="56"/>
-      <c r="B61" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="C61" s="49"/>
-      <c r="D61" s="49"/>
-      <c r="E61" s="49"/>
-      <c r="F61" s="50">
+    <row r="61" spans="1:61" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="55"/>
+      <c r="B61" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="C61" s="48"/>
+      <c r="D61" s="48"/>
+      <c r="E61" s="48"/>
+      <c r="F61" s="49">
         <v>210</v>
       </c>
       <c r="G61" s="25">
@@ -10397,15 +10555,15 @@
         <v>21193373.567737397</v>
       </c>
     </row>
-    <row r="62" spans="1:61">
+    <row r="62" spans="1:61" x14ac:dyDescent="0.3">
       <c r="BB62" s="10"/>
       <c r="BC62" s="10"/>
     </row>
-    <row r="63" spans="1:61">
+    <row r="63" spans="1:61" x14ac:dyDescent="0.3">
       <c r="BB63" s="10"/>
       <c r="BC63" s="10"/>
     </row>
-    <row r="64" spans="1:61">
+    <row r="64" spans="1:61" x14ac:dyDescent="0.3">
       <c r="G64" s="24"/>
       <c r="H64" s="24"/>
       <c r="I64" s="24"/>
@@ -10456,7 +10614,7 @@
       <c r="BB64" s="10"/>
       <c r="BC64" s="10"/>
     </row>
-    <row r="65" spans="7:55">
+    <row r="65" spans="7:55" x14ac:dyDescent="0.3">
       <c r="G65" s="24"/>
       <c r="H65" s="24"/>
       <c r="I65" s="24"/>
@@ -10507,7 +10665,7 @@
       <c r="BB65" s="10"/>
       <c r="BC65" s="10"/>
     </row>
-    <row r="66" spans="7:55">
+    <row r="66" spans="7:55" x14ac:dyDescent="0.3">
       <c r="G66" s="24"/>
       <c r="H66" s="24"/>
       <c r="I66" s="24"/>
@@ -10558,35 +10716,35 @@
       <c r="BB66" s="10"/>
       <c r="BC66" s="10"/>
     </row>
-    <row r="67" spans="7:55">
+    <row r="67" spans="7:55" x14ac:dyDescent="0.3">
       <c r="BB67" s="10"/>
       <c r="BC67" s="10"/>
     </row>
-    <row r="68" spans="7:55">
+    <row r="68" spans="7:55" x14ac:dyDescent="0.3">
       <c r="BB68" s="10"/>
       <c r="BC68" s="10"/>
     </row>
-    <row r="69" spans="7:55">
+    <row r="69" spans="7:55" x14ac:dyDescent="0.3">
       <c r="BB69" s="10"/>
       <c r="BC69" s="10"/>
     </row>
-    <row r="70" spans="7:55">
+    <row r="70" spans="7:55" x14ac:dyDescent="0.3">
       <c r="BB70" s="10"/>
       <c r="BC70" s="10"/>
     </row>
-    <row r="71" spans="7:55">
+    <row r="71" spans="7:55" x14ac:dyDescent="0.3">
       <c r="BB71" s="10"/>
       <c r="BC71" s="10"/>
     </row>
-    <row r="72" spans="7:55">
+    <row r="72" spans="7:55" x14ac:dyDescent="0.3">
       <c r="BB72" s="10"/>
       <c r="BC72" s="10"/>
     </row>
-    <row r="73" spans="7:55">
+    <row r="73" spans="7:55" x14ac:dyDescent="0.3">
       <c r="BB73" s="27"/>
       <c r="BC73" s="27"/>
     </row>
-    <row r="75" spans="7:55">
+    <row r="75" spans="7:55" x14ac:dyDescent="0.3">
       <c r="BB75" s="27"/>
     </row>
   </sheetData>
@@ -10608,16 +10766,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AT46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:AT46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:46">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>8861.6062989934399</v>
       </c>
@@ -10757,7 +10915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:46">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -10897,7 +11055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:46">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -11037,7 +11195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:46">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>198.42917976327374</v>
       </c>
@@ -11177,7 +11335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:46">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -11317,7 +11475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:46">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -11457,7 +11615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:46">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -11597,7 +11755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:46">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -11737,7 +11895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:46">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -11877,7 +12035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:46">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -12017,7 +12175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:46">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>167.36136096097101</v>
       </c>
@@ -12157,7 +12315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:46">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7.3607237068600462</v>
       </c>
@@ -12297,7 +12455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:46">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7.4628099864028048</v>
       </c>
@@ -12437,7 +12595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:46">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -12577,7 +12735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:46">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -12717,7 +12875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:46">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -12857,7 +13015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:46">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -12997,7 +13155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:46">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -13137,7 +13295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:46">
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -13277,7 +13435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:46">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -13417,7 +13575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:46">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -13557,7 +13715,7 @@
         <v>80.907912788144742</v>
       </c>
     </row>
-    <row r="22" spans="1:46">
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10.195193479324947</v>
       </c>
@@ -13697,7 +13855,7 @@
         <v>1.0173042994020538</v>
       </c>
     </row>
-    <row r="23" spans="1:46">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -13837,7 +13995,7 @@
         <v>1799.8948576795513</v>
       </c>
     </row>
-    <row r="24" spans="1:46">
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.13753138487654773</v>
       </c>
@@ -13977,7 +14135,7 @@
         <v>35.776449776967574</v>
       </c>
     </row>
-    <row r="25" spans="1:46">
+    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>10037.727475429792</v>
       </c>
@@ -14117,7 +14275,7 @@
         <v>1.6804829043534635</v>
       </c>
     </row>
-    <row r="26" spans="1:46">
+    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -14257,7 +14415,7 @@
         <v>473.88705701977278</v>
       </c>
     </row>
-    <row r="27" spans="1:46">
+    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25.248656006862156</v>
       </c>
@@ -14397,7 +14555,7 @@
         <v>28.151807722860436</v>
       </c>
     </row>
-    <row r="28" spans="1:46">
+    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1.3663484077668809E-3</v>
       </c>
@@ -14537,7 +14695,7 @@
         <v>140.9219867727997</v>
       </c>
     </row>
-    <row r="29" spans="1:46">
+    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0</v>
       </c>
@@ -14677,7 +14835,7 @@
         <v>1159.5479036723546</v>
       </c>
     </row>
-    <row r="30" spans="1:46">
+    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>39.188201125785341</v>
       </c>
@@ -14817,7 +14975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:46">
+    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>526.83456634863876</v>
       </c>
@@ -14957,7 +15115,7 @@
         <v>6722.5246103916734</v>
       </c>
     </row>
-    <row r="32" spans="1:46">
+    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>6.895583919607355</v>
       </c>
@@ -15097,7 +15255,7 @@
         <v>2793.8578664372521</v>
       </c>
     </row>
-    <row r="33" spans="1:46">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1363.6900191968193</v>
       </c>
@@ -15237,7 +15395,7 @@
         <v>2342.1529227521382</v>
       </c>
     </row>
-    <row r="34" spans="1:46">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0</v>
       </c>
@@ -15377,7 +15535,7 @@
         <v>168.92327815653346</v>
       </c>
     </row>
-    <row r="35" spans="1:46">
+    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>65.695009855384697</v>
       </c>
@@ -15517,7 +15675,7 @@
         <v>51.784511946661127</v>
       </c>
     </row>
-    <row r="36" spans="1:46">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0</v>
       </c>
@@ -15657,7 +15815,7 @@
         <v>8.7656001355610194</v>
       </c>
     </row>
-    <row r="37" spans="1:46">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0</v>
       </c>
@@ -15797,7 +15955,7 @@
         <v>23.745523719354804</v>
       </c>
     </row>
-    <row r="38" spans="1:46">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0</v>
       </c>
@@ -15937,7 +16095,7 @@
         <v>2120.2397506983011</v>
       </c>
     </row>
-    <row r="39" spans="1:46">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>426.16427395526205</v>
       </c>
@@ -16077,7 +16235,7 @@
         <v>1350.4418460618122</v>
       </c>
     </row>
-    <row r="40" spans="1:46">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>339.9277834403058</v>
       </c>
@@ -16217,7 +16375,7 @@
         <v>5725.9234574646143</v>
       </c>
     </row>
-    <row r="41" spans="1:46">
+    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0</v>
       </c>
@@ -16357,7 +16515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:46">
+    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0</v>
       </c>
@@ -16497,7 +16655,7 @@
         <v>296.5114967946231</v>
       </c>
     </row>
-    <row r="43" spans="1:46">
+    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>531.34232561756323</v>
       </c>
@@ -16637,7 +16795,7 @@
         <v>2163.0188206542289</v>
       </c>
     </row>
-    <row r="44" spans="1:46">
+    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>0</v>
       </c>
@@ -16777,7 +16935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:46">
+    <row r="45" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>0</v>
       </c>
@@ -16917,7 +17075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:46">
+    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>11.547562687172201</v>
       </c>
@@ -17063,16 +17221,864 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:B46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:AT3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:AT3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>29.160240023582634</v>
+      </c>
+      <c r="B1">
+        <v>183.44688654753242</v>
+      </c>
+      <c r="C1">
+        <v>220.81716159691524</v>
+      </c>
+      <c r="D1">
+        <v>325.68762077872253</v>
+      </c>
+      <c r="E1">
+        <v>51.062419352709341</v>
+      </c>
+      <c r="F1">
+        <v>62.712572714240338</v>
+      </c>
+      <c r="G1">
+        <v>6.9988232557722547</v>
+      </c>
+      <c r="H1">
+        <v>91.11638018366429</v>
+      </c>
+      <c r="I1">
+        <v>176.89015298133239</v>
+      </c>
+      <c r="J1">
+        <v>29.760795209965679</v>
+      </c>
+      <c r="K1">
+        <v>196.39225531598026</v>
+      </c>
+      <c r="L1">
+        <v>1047.8976325572553</v>
+      </c>
+      <c r="M1">
+        <v>62.505461804600657</v>
+      </c>
+      <c r="N1">
+        <v>5.8970018267880677</v>
+      </c>
+      <c r="O1">
+        <v>40.941917371214593</v>
+      </c>
+      <c r="P1">
+        <v>492.61340046102941</v>
+      </c>
+      <c r="Q1">
+        <v>128.9520010414335</v>
+      </c>
+      <c r="R1">
+        <v>255.34643170776735</v>
+      </c>
+      <c r="S1">
+        <v>13.209529055923799</v>
+      </c>
+      <c r="T1">
+        <v>690.12723105572491</v>
+      </c>
+      <c r="U1">
+        <v>202.34712655683941</v>
+      </c>
+      <c r="V1">
+        <v>201.49021089574464</v>
+      </c>
+      <c r="W1">
+        <v>16.772658795379343</v>
+      </c>
+      <c r="X1">
+        <v>14.965515938433537</v>
+      </c>
+      <c r="Y1">
+        <v>21.465947593652714</v>
+      </c>
+      <c r="Z1">
+        <v>167.31070828709449</v>
+      </c>
+      <c r="AA1">
+        <v>843.49762523207312</v>
+      </c>
+      <c r="AB1">
+        <v>1153.5978946439943</v>
+      </c>
+      <c r="AC1">
+        <v>167.26607032345311</v>
+      </c>
+      <c r="AD1">
+        <v>378.3044734088196</v>
+      </c>
+      <c r="AE1">
+        <v>79.513491272980914</v>
+      </c>
+      <c r="AF1">
+        <v>44.494095833498683</v>
+      </c>
+      <c r="AG1">
+        <v>55.759470229308747</v>
+      </c>
+      <c r="AH1">
+        <v>37.756377387729636</v>
+      </c>
+      <c r="AI1">
+        <v>57.160279205960222</v>
+      </c>
+      <c r="AJ1">
+        <v>78.755175201731745</v>
+      </c>
+      <c r="AK1">
+        <v>183.85368750550228</v>
+      </c>
+      <c r="AL1">
+        <v>432.1885305633549</v>
+      </c>
+      <c r="AM1">
+        <v>91.996368243112471</v>
+      </c>
+      <c r="AN1">
+        <v>55.005128955057089</v>
+      </c>
+      <c r="AO1">
+        <v>1422.0934260312774</v>
+      </c>
+      <c r="AP1">
+        <v>3093.1218083646627</v>
+      </c>
+      <c r="AQ1">
+        <v>2054.7801189350662</v>
+      </c>
+      <c r="AR1">
+        <v>1207.3154752639489</v>
+      </c>
+      <c r="AS1">
+        <v>2694.1912807056979</v>
+      </c>
+      <c r="AT1">
+        <v>2328.3677496404816</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1844809.6525243714</v>
+      </c>
+      <c r="B2">
+        <v>305018.00206966395</v>
+      </c>
+      <c r="C2">
+        <v>531517.9258165647</v>
+      </c>
+      <c r="D2">
+        <v>244432.53501751443</v>
+      </c>
+      <c r="E2">
+        <v>404425.20883534895</v>
+      </c>
+      <c r="F2">
+        <v>271609.55343070888</v>
+      </c>
+      <c r="G2">
+        <v>466893.65811812301</v>
+      </c>
+      <c r="H2">
+        <v>299855.91686051048</v>
+      </c>
+      <c r="I2">
+        <v>184707.23583510917</v>
+      </c>
+      <c r="J2">
+        <v>92269.830805187987</v>
+      </c>
+      <c r="K2">
+        <v>139586.59325139635</v>
+      </c>
+      <c r="L2">
+        <v>931936.84691651422</v>
+      </c>
+      <c r="M2">
+        <v>982878.03903014748</v>
+      </c>
+      <c r="N2">
+        <v>205180.65427288899</v>
+      </c>
+      <c r="O2">
+        <v>8.5051965470483992E-12</v>
+      </c>
+      <c r="P2">
+        <v>333597.27133007167</v>
+      </c>
+      <c r="Q2">
+        <v>2.2737367544323206E-13</v>
+      </c>
+      <c r="R2">
+        <v>22047.010898529581</v>
+      </c>
+      <c r="S2">
+        <v>427124.82315682713</v>
+      </c>
+      <c r="T2">
+        <v>286364.09493425034</v>
+      </c>
+      <c r="U2">
+        <v>6670.2382022151114</v>
+      </c>
+      <c r="V2">
+        <v>28433.896887057974</v>
+      </c>
+      <c r="W2">
+        <v>194749.82995830892</v>
+      </c>
+      <c r="X2">
+        <v>73739.709334466403</v>
+      </c>
+      <c r="Y2">
+        <v>538230.5296810146</v>
+      </c>
+      <c r="Z2">
+        <v>20267.20017561538</v>
+      </c>
+      <c r="AA2">
+        <v>14156.671688551975</v>
+      </c>
+      <c r="AB2">
+        <v>3557.4687790829767</v>
+      </c>
+      <c r="AC2">
+        <v>175521.89015998042</v>
+      </c>
+      <c r="AD2">
+        <v>980256.9311505775</v>
+      </c>
+      <c r="AE2">
+        <v>2897930.8825009265</v>
+      </c>
+      <c r="AF2">
+        <v>820585.15076984349</v>
+      </c>
+      <c r="AG2">
+        <v>1622135.3571647599</v>
+      </c>
+      <c r="AH2">
+        <v>-6.3948846218409017E-14</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>-1.2789769243681803E-13</v>
+      </c>
+      <c r="AK2">
+        <v>83049.247697726722</v>
+      </c>
+      <c r="AL2">
+        <v>118919.91267818987</v>
+      </c>
+      <c r="AM2">
+        <v>241919.46944296549</v>
+      </c>
+      <c r="AN2">
+        <v>692546.64744242909</v>
+      </c>
+      <c r="AO2">
+        <v>951363.36544807919</v>
+      </c>
+      <c r="AP2">
+        <v>303066.84562873968</v>
+      </c>
+      <c r="AQ2">
+        <v>216242.44852795862</v>
+      </c>
+      <c r="AR2">
+        <v>487481.68928325601</v>
+      </c>
+      <c r="AS2">
+        <v>201510.32337805978</v>
+      </c>
+      <c r="AT2">
+        <v>168624.86887955887</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2.0453348202261328</v>
+      </c>
+      <c r="B3">
+        <v>37.427335068308501</v>
+      </c>
+      <c r="C3">
+        <v>1.2938222803974526</v>
+      </c>
+      <c r="D3">
+        <v>18.617582025273734</v>
+      </c>
+      <c r="E3">
+        <v>1.2377285742885573</v>
+      </c>
+      <c r="F3">
+        <v>3.350133306457304</v>
+      </c>
+      <c r="G3">
+        <v>1.6813698602146159</v>
+      </c>
+      <c r="H3">
+        <v>13.86669542333995</v>
+      </c>
+      <c r="I3">
+        <v>4.3700694865296841</v>
+      </c>
+      <c r="J3">
+        <v>1.85544763489308</v>
+      </c>
+      <c r="K3">
+        <v>5.5253348315704356</v>
+      </c>
+      <c r="L3">
+        <v>155.49930240645349</v>
+      </c>
+      <c r="M3">
+        <v>5.3992871600533707</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0.41068806121918211</v>
+      </c>
+      <c r="P3">
+        <v>6.4445060827324472</v>
+      </c>
+      <c r="Q3">
+        <v>5.8884779251121318</v>
+      </c>
+      <c r="R3">
+        <v>4.6786479352062731</v>
+      </c>
+      <c r="S3">
+        <v>0.46358794324572072</v>
+      </c>
+      <c r="T3">
+        <v>86.938697688367711</v>
+      </c>
+      <c r="U3">
+        <v>0.49937937107461439</v>
+      </c>
+      <c r="V3">
+        <v>0.44143025347544729</v>
+      </c>
+      <c r="W3">
+        <v>1.6915332094048707</v>
+      </c>
+      <c r="X3">
+        <v>0.13034918902177609</v>
+      </c>
+      <c r="Y3">
+        <v>0.13247034667632221</v>
+      </c>
+      <c r="Z3">
+        <v>0.77208502796754452</v>
+      </c>
+      <c r="AA3">
+        <v>15.367424234555966</v>
+      </c>
+      <c r="AB3">
+        <v>249.89451877644453</v>
+      </c>
+      <c r="AC3">
+        <v>15.63750054876223</v>
+      </c>
+      <c r="AD3">
+        <v>8.6330912389944761</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0.72360234806930757</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0.70545432437455702</v>
+      </c>
+      <c r="AI3">
+        <v>0.20596238252096788</v>
+      </c>
+      <c r="AJ3">
+        <v>4.1980340114189261</v>
+      </c>
+      <c r="AK3">
+        <v>58.396935692287528</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>9.8731375582274808E-2</v>
+      </c>
+      <c r="AN3">
+        <v>9.0762131275087565</v>
+      </c>
+      <c r="AO3">
+        <v>0</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -17086,7 +18092,7 @@
         <v>2022123.5222451445</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>7106.3525191046429</v>
       </c>
@@ -17100,7 +18106,7 @@
         <v>354537.05371124647</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20616.882248878588</v>
       </c>
@@ -17114,7 +18120,7 @@
         <v>592872.11684652371</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3777.3647616431222</v>
       </c>
@@ -17128,7 +18134,7 @@
         <v>279805.97444075253</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>60718.706309664085</v>
       </c>
@@ -17142,7 +18148,7 @@
         <v>490272.85165061796</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>834.1504266472831</v>
       </c>
@@ -17156,7 +18162,7 @@
         <v>312347.16883912857</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8397.3398934086526</v>
       </c>
@@ -17170,7 +18176,7 @@
         <v>560387.82958212215</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>151796.76577416022</v>
       </c>
@@ -17184,7 +18190,7 @@
         <v>335363.57882716419</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2085.3760666182075</v>
       </c>
@@ -17198,7 +18204,7 @@
         <v>239939.83323308284</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20993.349733521634</v>
       </c>
@@ -17212,7 +18218,7 @@
         <v>107225.24484326984</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>17622.062258684487</v>
       </c>
@@ -17226,7 +18232,7 @@
         <v>186722.33868726171</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12133.673929197423</v>
       </c>
@@ -17240,7 +18246,7 @@
         <v>1023674.1427694296</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2036.7313916362416</v>
       </c>
@@ -17254,7 +18260,7 @@
         <v>1086787.1260668619</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>24343.487349670955</v>
       </c>
@@ -17268,7 +18274,7 @@
         <v>243265.62882683545</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>16367.875638497266</v>
       </c>
@@ -17282,7 +18288,7 @@
         <v>102747.50329169189</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13189.051877719212</v>
       </c>
@@ -17296,7 +18302,7 @@
         <v>364557.90263297054</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -17310,7 +18316,7 @@
         <v>2006.1344505049096</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14997.364795527086</v>
       </c>
@@ -17324,7 +18330,7 @@
         <v>67335.299627857836</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1233.0367614994068</v>
       </c>
@@ -17338,7 +18344,7 @@
         <v>522758.14643934241</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>22304.64097216594</v>
       </c>
@@ -17352,7 +18358,7 @@
         <v>567150.87550378067</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>84106.643043819742</v>
       </c>
@@ -17366,7 +18372,7 @@
         <v>57284.404441600156</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>14477.078271806928</v>
       </c>
@@ -17380,7 +18386,7 @@
         <v>33269.221326199448</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>17924.505237920192</v>
       </c>
@@ -17394,7 +18400,7 @@
         <v>532003.20716412133</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>26236.39970223009</v>
       </c>
@@ -17408,7 +18414,7 @@
         <v>86808.719166688374</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>8292.8595914908637</v>
       </c>
@@ -17422,7 +18428,7 @@
         <v>593688.57871703629</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5095.0009578937752</v>
       </c>
@@ -17436,7 +18442,7 @@
         <v>35801.564525019923</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>17044.671116507237</v>
       </c>
@@ -17450,7 +18456,7 @@
         <v>65340.544789178406</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>439.91706070647791</v>
       </c>
@@ -17464,7 +18470,7 @@
         <v>44276.988219932166</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>11416.693719680612</v>
       </c>
@@ -17478,7 +18484,7 @@
         <v>207749.49057762144</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>20035.261134963774</v>
       </c>
@@ -17492,7 +18498,7 @@
         <v>1276761.8937704677</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1199.1969875989084</v>
       </c>
@@ -17506,7 +18512,7 @@
         <v>3355418.5485547255</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0</v>
       </c>
@@ -17520,7 +18526,7 @@
         <v>971282.50355638657</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>25743.607994804082</v>
       </c>
@@ -17534,7 +18540,7 @@
         <v>1791469.1228406865</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>15722.804948519024</v>
       </c>
@@ -17548,7 +18554,7 @@
         <v>3096.8014050077618</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1636.9990624366053</v>
       </c>
@@ -17562,7 +18568,7 @@
         <v>3876.6172128396856</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>145.9340249458989</v>
       </c>
@@ -17576,7 +18582,7 @@
         <v>1089.3680417818402</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>78.25447714490231</v>
       </c>
@@ -17590,7 +18596,7 @@
         <v>113375.00250981956</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>11095.21586762588</v>
       </c>
@@ -17604,7 +18610,7 @@
         <v>163286.41974900721</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>41073.025571729813</v>
       </c>
@@ -17618,7 +18624,7 @@
         <v>271476.31340236048</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>23313.489231574549</v>
       </c>
@@ -17632,7 +18638,7 @@
         <v>794172.46056213905</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2292.6446817587594</v>
       </c>
@@ -17646,7 +18652,7 @@
         <v>1230058.266876718</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>14944.490148807561</v>
       </c>
@@ -17660,7 +18666,7 @@
         <v>364635.6810584357</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>19032.757833161511</v>
       </c>
@@ -17674,7 +18680,7 @@
         <v>319611.23684705497</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2988.8980297615121</v>
       </c>
@@ -17688,7 +18694,7 @@
         <v>1040514.6088890161</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>458.52893635175195</v>
       </c>
@@ -17702,7 +18708,7 @@
         <v>260447.47925833619</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>41073.025571729813</v>
       </c>
@@ -17714,854 +18720,6 @@
       </c>
       <c r="D46">
         <v>221823.05762770658</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B46"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>39</v>
-      </c>
-      <c r="B34" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
-        <v>40</v>
-      </c>
-      <c r="B35" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
-        <v>41</v>
-      </c>
-      <c r="B36" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s">
-        <v>42</v>
-      </c>
-      <c r="B37" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
-        <v>43</v>
-      </c>
-      <c r="B38" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B42" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" t="s">
-        <v>49</v>
-      </c>
-      <c r="B44" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" t="s">
-        <v>51</v>
-      </c>
-      <c r="B46" t="s">
-        <v>69</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AT3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:AT3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
-  <sheetData>
-    <row r="1" spans="1:46">
-      <c r="A1">
-        <v>29.160240023582634</v>
-      </c>
-      <c r="B1">
-        <v>183.44688654753242</v>
-      </c>
-      <c r="C1">
-        <v>220.81716159691524</v>
-      </c>
-      <c r="D1">
-        <v>325.68762077872253</v>
-      </c>
-      <c r="E1">
-        <v>51.062419352709341</v>
-      </c>
-      <c r="F1">
-        <v>62.712572714240338</v>
-      </c>
-      <c r="G1">
-        <v>6.9988232557722547</v>
-      </c>
-      <c r="H1">
-        <v>91.11638018366429</v>
-      </c>
-      <c r="I1">
-        <v>176.89015298133239</v>
-      </c>
-      <c r="J1">
-        <v>29.760795209965679</v>
-      </c>
-      <c r="K1">
-        <v>196.39225531598026</v>
-      </c>
-      <c r="L1">
-        <v>1047.8976325572553</v>
-      </c>
-      <c r="M1">
-        <v>62.505461804600657</v>
-      </c>
-      <c r="N1">
-        <v>5.8970018267880677</v>
-      </c>
-      <c r="O1">
-        <v>40.941917371214593</v>
-      </c>
-      <c r="P1">
-        <v>492.61340046102941</v>
-      </c>
-      <c r="Q1">
-        <v>128.9520010414335</v>
-      </c>
-      <c r="R1">
-        <v>255.34643170776735</v>
-      </c>
-      <c r="S1">
-        <v>13.209529055923799</v>
-      </c>
-      <c r="T1">
-        <v>690.12723105572491</v>
-      </c>
-      <c r="U1">
-        <v>202.34712655683941</v>
-      </c>
-      <c r="V1">
-        <v>201.49021089574464</v>
-      </c>
-      <c r="W1">
-        <v>16.772658795379343</v>
-      </c>
-      <c r="X1">
-        <v>14.965515938433537</v>
-      </c>
-      <c r="Y1">
-        <v>21.465947593652714</v>
-      </c>
-      <c r="Z1">
-        <v>167.31070828709449</v>
-      </c>
-      <c r="AA1">
-        <v>843.49762523207312</v>
-      </c>
-      <c r="AB1">
-        <v>1153.5978946439943</v>
-      </c>
-      <c r="AC1">
-        <v>167.26607032345311</v>
-      </c>
-      <c r="AD1">
-        <v>378.3044734088196</v>
-      </c>
-      <c r="AE1">
-        <v>79.513491272980914</v>
-      </c>
-      <c r="AF1">
-        <v>44.494095833498683</v>
-      </c>
-      <c r="AG1">
-        <v>55.759470229308747</v>
-      </c>
-      <c r="AH1">
-        <v>37.756377387729636</v>
-      </c>
-      <c r="AI1">
-        <v>57.160279205960222</v>
-      </c>
-      <c r="AJ1">
-        <v>78.755175201731745</v>
-      </c>
-      <c r="AK1">
-        <v>183.85368750550228</v>
-      </c>
-      <c r="AL1">
-        <v>432.1885305633549</v>
-      </c>
-      <c r="AM1">
-        <v>91.996368243112471</v>
-      </c>
-      <c r="AN1">
-        <v>55.005128955057089</v>
-      </c>
-      <c r="AO1">
-        <v>1422.0934260312774</v>
-      </c>
-      <c r="AP1">
-        <v>3093.1218083646627</v>
-      </c>
-      <c r="AQ1">
-        <v>2054.7801189350662</v>
-      </c>
-      <c r="AR1">
-        <v>1207.3154752639489</v>
-      </c>
-      <c r="AS1">
-        <v>2694.1912807056979</v>
-      </c>
-      <c r="AT1">
-        <v>2328.3677496404816</v>
-      </c>
-    </row>
-    <row r="2" spans="1:46">
-      <c r="A2">
-        <v>1844809.6525243714</v>
-      </c>
-      <c r="B2">
-        <v>305018.00206966395</v>
-      </c>
-      <c r="C2">
-        <v>531517.9258165647</v>
-      </c>
-      <c r="D2">
-        <v>244432.53501751443</v>
-      </c>
-      <c r="E2">
-        <v>404425.20883534895</v>
-      </c>
-      <c r="F2">
-        <v>271609.55343070888</v>
-      </c>
-      <c r="G2">
-        <v>466893.65811812301</v>
-      </c>
-      <c r="H2">
-        <v>299855.91686051048</v>
-      </c>
-      <c r="I2">
-        <v>184707.23583510917</v>
-      </c>
-      <c r="J2">
-        <v>92269.830805187987</v>
-      </c>
-      <c r="K2">
-        <v>139586.59325139635</v>
-      </c>
-      <c r="L2">
-        <v>931936.84691651422</v>
-      </c>
-      <c r="M2">
-        <v>982878.03903014748</v>
-      </c>
-      <c r="N2">
-        <v>205180.65427288899</v>
-      </c>
-      <c r="O2">
-        <v>8.5051965470483992E-12</v>
-      </c>
-      <c r="P2">
-        <v>333597.27133007167</v>
-      </c>
-      <c r="Q2">
-        <v>2.2737367544323206E-13</v>
-      </c>
-      <c r="R2">
-        <v>22047.010898529581</v>
-      </c>
-      <c r="S2">
-        <v>427124.82315682713</v>
-      </c>
-      <c r="T2">
-        <v>286364.09493425034</v>
-      </c>
-      <c r="U2">
-        <v>6670.2382022151114</v>
-      </c>
-      <c r="V2">
-        <v>28433.896887057974</v>
-      </c>
-      <c r="W2">
-        <v>194749.82995830892</v>
-      </c>
-      <c r="X2">
-        <v>73739.709334466403</v>
-      </c>
-      <c r="Y2">
-        <v>538230.5296810146</v>
-      </c>
-      <c r="Z2">
-        <v>20267.20017561538</v>
-      </c>
-      <c r="AA2">
-        <v>14156.671688551975</v>
-      </c>
-      <c r="AB2">
-        <v>3557.4687790829767</v>
-      </c>
-      <c r="AC2">
-        <v>175521.89015998042</v>
-      </c>
-      <c r="AD2">
-        <v>980256.9311505775</v>
-      </c>
-      <c r="AE2">
-        <v>2897930.8825009265</v>
-      </c>
-      <c r="AF2">
-        <v>820585.15076984349</v>
-      </c>
-      <c r="AG2">
-        <v>1622135.3571647599</v>
-      </c>
-      <c r="AH2">
-        <v>-6.3948846218409017E-14</v>
-      </c>
-      <c r="AI2">
-        <v>0</v>
-      </c>
-      <c r="AJ2">
-        <v>-1.2789769243681803E-13</v>
-      </c>
-      <c r="AK2">
-        <v>83049.247697726722</v>
-      </c>
-      <c r="AL2">
-        <v>118919.91267818987</v>
-      </c>
-      <c r="AM2">
-        <v>241919.46944296549</v>
-      </c>
-      <c r="AN2">
-        <v>692546.64744242909</v>
-      </c>
-      <c r="AO2">
-        <v>951363.36544807919</v>
-      </c>
-      <c r="AP2">
-        <v>303066.84562873968</v>
-      </c>
-      <c r="AQ2">
-        <v>216242.44852795862</v>
-      </c>
-      <c r="AR2">
-        <v>487481.68928325601</v>
-      </c>
-      <c r="AS2">
-        <v>201510.32337805978</v>
-      </c>
-      <c r="AT2">
-        <v>168624.86887955887</v>
-      </c>
-    </row>
-    <row r="3" spans="1:46">
-      <c r="A3">
-        <v>2.0453348202261328</v>
-      </c>
-      <c r="B3">
-        <v>37.427335068308501</v>
-      </c>
-      <c r="C3">
-        <v>1.2938222803974526</v>
-      </c>
-      <c r="D3">
-        <v>18.617582025273734</v>
-      </c>
-      <c r="E3">
-        <v>1.2377285742885573</v>
-      </c>
-      <c r="F3">
-        <v>3.350133306457304</v>
-      </c>
-      <c r="G3">
-        <v>1.6813698602146159</v>
-      </c>
-      <c r="H3">
-        <v>13.86669542333995</v>
-      </c>
-      <c r="I3">
-        <v>4.3700694865296841</v>
-      </c>
-      <c r="J3">
-        <v>1.85544763489308</v>
-      </c>
-      <c r="K3">
-        <v>5.5253348315704356</v>
-      </c>
-      <c r="L3">
-        <v>155.49930240645349</v>
-      </c>
-      <c r="M3">
-        <v>5.3992871600533707</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0.41068806121918211</v>
-      </c>
-      <c r="P3">
-        <v>6.4445060827324472</v>
-      </c>
-      <c r="Q3">
-        <v>5.8884779251121318</v>
-      </c>
-      <c r="R3">
-        <v>4.6786479352062731</v>
-      </c>
-      <c r="S3">
-        <v>0.46358794324572072</v>
-      </c>
-      <c r="T3">
-        <v>86.938697688367711</v>
-      </c>
-      <c r="U3">
-        <v>0.49937937107461439</v>
-      </c>
-      <c r="V3">
-        <v>0.44143025347544729</v>
-      </c>
-      <c r="W3">
-        <v>1.6915332094048707</v>
-      </c>
-      <c r="X3">
-        <v>0.13034918902177609</v>
-      </c>
-      <c r="Y3">
-        <v>0.13247034667632221</v>
-      </c>
-      <c r="Z3">
-        <v>0.77208502796754452</v>
-      </c>
-      <c r="AA3">
-        <v>15.367424234555966</v>
-      </c>
-      <c r="AB3">
-        <v>249.89451877644453</v>
-      </c>
-      <c r="AC3">
-        <v>15.63750054876223</v>
-      </c>
-      <c r="AD3">
-        <v>8.6330912389944761</v>
-      </c>
-      <c r="AE3">
-        <v>0</v>
-      </c>
-      <c r="AF3">
-        <v>0.72360234806930757</v>
-      </c>
-      <c r="AG3">
-        <v>0</v>
-      </c>
-      <c r="AH3">
-        <v>0.70545432437455702</v>
-      </c>
-      <c r="AI3">
-        <v>0.20596238252096788</v>
-      </c>
-      <c r="AJ3">
-        <v>4.1980340114189261</v>
-      </c>
-      <c r="AK3">
-        <v>58.396935692287528</v>
-      </c>
-      <c r="AL3">
-        <v>0</v>
-      </c>
-      <c r="AM3">
-        <v>9.8731375582274808E-2</v>
-      </c>
-      <c r="AN3">
-        <v>9.0762131275087565</v>
-      </c>
-      <c r="AO3">
-        <v>0</v>
-      </c>
-      <c r="AP3">
-        <v>0</v>
-      </c>
-      <c r="AQ3">
-        <v>0</v>
-      </c>
-      <c r="AR3">
-        <v>0</v>
-      </c>
-      <c r="AS3">
-        <v>0</v>
-      </c>
-      <c r="AT3">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -18570,33 +18728,33 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>